<commit_message>
Commit before massive changes
</commit_message>
<xml_diff>
--- a/resources/data/OfficerRegistration.xlsx
+++ b/resources/data/OfficerRegistration.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5a02774ed8d28bca/Documents/GitHub/SC2002-BTO-V3/resources/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="8_{B400D56E-B4EC-45DD-8386-64B1F51077C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{692B4C10-62EA-474C-A890-1155FCC299D6}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="8_{B400D56E-B4EC-45DD-8386-64B1F51077C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{743AA7E9-F384-41DE-83E9-B6746D3228FE}"/>
   <bookViews>
-    <workbookView xWindow="7020" yWindow="1013" windowWidth="14580" windowHeight="11767" xr2:uid="{E928912E-6233-4515-AF28-B6354C627B77}"/>
+    <workbookView xWindow="1710" yWindow="1013" windowWidth="14580" windowHeight="11767" xr2:uid="{E928912E-6233-4515-AF28-B6354C627B77}"/>
   </bookViews>
   <sheets>
     <sheet name="OfficerRegistration" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Officer Registration ID</t>
   </si>
@@ -38,12 +38,6 @@
   </si>
   <si>
     <t>T2109876H</t>
-  </si>
-  <si>
-    <t>Successful</t>
-  </si>
-  <si>
-    <t>T1234567J</t>
   </si>
   <si>
     <t>Pending</t>
@@ -908,10 +902,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFD7A5E9-85EC-41F1-82F3-D8105BF1EF69}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="A2" sqref="A2:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -936,38 +930,21 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A2">
-        <v>1</v>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1.0</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="C2">
-        <v>2</v>
+      <c r="C2" t="n">
+        <v>4.0</v>
       </c>
       <c r="D2" t="s">
         <v>6</v>
       </c>
-      <c r="E2">
-        <v>45767.794050636578</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="D3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" t="n">
-        <v>45767.89375944444</v>
+      <c r="E2" t="n">
+        <v>45768.5425244213</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
DEV 4.1 - Officer Registration Management
</commit_message>
<xml_diff>
--- a/resources/data/OfficerRegistration.xlsx
+++ b/resources/data/OfficerRegistration.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5a02774ed8d28bca/Documents/GitHub/SC2002-BTO-V3/resources/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/racshanyaa/Documents/GitHub/SC2002-BTO-V3/resources/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="11" documentId="8_{B400D56E-B4EC-45DD-8386-64B1F51077C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{743AA7E9-F384-41DE-83E9-B6746D3228FE}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EAEB46D-5859-E941-A1E8-05E11BF839E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1710" yWindow="1013" windowWidth="14580" windowHeight="11767" xr2:uid="{E928912E-6233-4515-AF28-B6354C627B77}"/>
+    <workbookView xWindow="1720" yWindow="1020" windowWidth="14580" windowHeight="11760" xr2:uid="{E928912E-6233-4515-AF28-B6354C627B77}"/>
   </bookViews>
   <sheets>
     <sheet name="OfficerRegistration" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
   <si>
     <t>Officer Registration ID</t>
   </si>
@@ -41,6 +41,9 @@
   </si>
   <si>
     <t>Pending</t>
+  </si>
+  <si>
+    <t>Approved</t>
   </si>
 </sst>
 </file>
@@ -904,16 +907,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFD7A5E9-85EC-41F1-82F3-D8105BF1EF69}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD3"/>
+    <sheetView tabSelected="1" zoomScale="191" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="17.86328125" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="17.83203125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -930,21 +933,21 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>1.0</v>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="n">
-        <v>4.0</v>
+      <c r="C2">
+        <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
-      <c r="E2" t="n">
-        <v>45768.5425244213</v>
+      <c r="E2">
+        <v>45768.542524421297</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
A new massive change
Some MVC done
</commit_message>
<xml_diff>
--- a/resources/data/OfficerRegistration.xlsx
+++ b/resources/data/OfficerRegistration.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="9">
   <si>
     <t>Officer Registration ID</t>
   </si>
@@ -44,6 +44,9 @@
   </si>
   <si>
     <t>Approved</t>
+  </si>
+  <si>
+    <t>T1234567J</t>
   </si>
 </sst>
 </file>
@@ -905,7 +908,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFD7A5E9-85EC-41F1-82F3-D8105BF1EF69}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="191" workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
@@ -950,6 +953,23 @@
         <v>45768.542524421297</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" t="n">
+        <v>45769.79456391204</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
DEV 6 - CLI Changes for Manager Application and Registration
</commit_message>
<xml_diff>
--- a/resources/data/OfficerRegistration.xlsx
+++ b/resources/data/OfficerRegistration.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/racshanyaa/Documents/GitHub/SC2002-BTO-V3/resources/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EAEB46D-5859-E941-A1E8-05E11BF839E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92779ECF-8BE2-7B4F-95CD-3800B081A860}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1720" yWindow="1020" windowWidth="14580" windowHeight="11760" xr2:uid="{E928912E-6233-4515-AF28-B6354C627B77}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Officer Registration ID</t>
   </si>
@@ -43,17 +43,16 @@
     <t>Pending</t>
   </si>
   <si>
-    <t>Approved</t>
+    <t>T1234567J</t>
   </si>
   <si>
-    <t>T1234567J</t>
+    <t>Successful</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -911,12 +910,12 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="191" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="17.83203125" collapsed="true"/>
+    <col min="1" max="1" width="17.83203125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
@@ -947,27 +946,27 @@
         <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E2">
         <v>45768.542524421297</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>1.0</v>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
         <v>8</v>
       </c>
-      <c r="C3" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="D3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" t="n">
-        <v>45769.79456391204</v>
+      <c r="E3">
+        <v>45769.794563912037</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changes to manager and officer
some minor and major UI stuff
</commit_message>
<xml_diff>
--- a/resources/data/OfficerRegistration.xlsx
+++ b/resources/data/OfficerRegistration.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/racshanyaa/Documents/GitHub/SC2002-BTO-V3/resources/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5a02774ed8d28bca/Documents/GitHub/SC2002-BTO-V3/resources/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92779ECF-8BE2-7B4F-95CD-3800B081A860}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{92779ECF-8BE2-7B4F-95CD-3800B081A860}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C9D4D970-DD01-4BCB-A92C-E85992FD4F99}"/>
   <bookViews>
-    <workbookView xWindow="1720" yWindow="1020" windowWidth="14580" windowHeight="11760" xr2:uid="{E928912E-6233-4515-AF28-B6354C627B77}"/>
+    <workbookView xWindow="1710" yWindow="1013" windowWidth="14580" windowHeight="11767" xr2:uid="{E928912E-6233-4515-AF28-B6354C627B77}"/>
   </bookViews>
   <sheets>
     <sheet name="OfficerRegistration" sheetId="1" r:id="rId1"/>
@@ -910,15 +910,15 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="191" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="17.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="17.796875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -935,7 +935,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>1</v>
       </c>
@@ -952,7 +952,7 @@
         <v>45768.542524421297</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>2</v>
       </c>
@@ -960,7 +960,7 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D3" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
DEV 7 - Manager Bug Fixes
</commit_message>
<xml_diff>
--- a/resources/data/OfficerRegistration.xlsx
+++ b/resources/data/OfficerRegistration.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/racshanyaa/Documents/GitHub/SC2002-BTO-V3/resources/data/"/>
     </mc:Choice>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Officer Registration ID</t>
   </si>
@@ -48,11 +48,15 @@
   <si>
     <t>Successful</t>
   </si>
+  <si>
+    <t>Unsuccessful</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -915,7 +919,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="17.83203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
@@ -946,7 +950,7 @@
         <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E2">
         <v>45768.542524421297</v>

</xml_diff>